<commit_message>
Added support for Hayden & Reynott on backend app
</commit_message>
<xml_diff>
--- a/public/shopify/Delivery_Institution_Details.xlsx
+++ b/public/shopify/Delivery_Institution_Details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="50">
   <si>
     <t xml:space="preserve">Delivery Institution</t>
   </si>
@@ -155,6 +155,21 @@
   </si>
   <si>
     <t xml:space="preserve">A, B, C, D, E, F, Reynott</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H&amp;R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plot 23 Gurugram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9,10,11,12,BA, MA, BOD, BCOM, BTECH, MCOM, BBA, MBA, BSC, BVOC, Creative Arts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A, B, C, D, E, F, H&amp;R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dwarka</t>
   </si>
 </sst>
 </file>
@@ -164,7 +179,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -215,8 +230,16 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -226,7 +249,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF3F3F3"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFEEEEEE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEEEEEE"/>
+        <bgColor rgb="FFF3F3F3"/>
       </patternFill>
     </fill>
   </fills>
@@ -264,7 +293,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -311,6 +340,50 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -342,7 +415,7 @@
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFEEEEEE"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
@@ -390,10 +463,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z29"/>
+  <dimension ref="A1:Z33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -906,12 +979,66 @@
       </c>
       <c r="G29" s="11"/>
     </row>
+    <row r="30" s="17" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="12"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="16"/>
+    </row>
+    <row r="31" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E31" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="F31" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="G31" s="21"/>
+      <c r="H31" s="22"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32" s="19"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="E2:E17"/>
     <mergeCell ref="F2:F17"/>
     <mergeCell ref="E19:E27"/>
     <mergeCell ref="F19:F27"/>
+    <mergeCell ref="E31:E32"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
changed H&R section logic and test cases
</commit_message>
<xml_diff>
--- a/public/shopify/Delivery_Institution_Details.xlsx
+++ b/public/shopify/Delivery_Institution_Details.xlsx
@@ -166,7 +166,7 @@
     <t xml:space="preserve">9,10,11,12,BA, MA, BOD, BCOM, BTECH, MCOM, BBA, MBA, BSC, BVOC, Creative Arts</t>
   </si>
   <si>
-    <t xml:space="preserve">A, B, C, D, E, F, H&amp;R</t>
+    <t xml:space="preserve"> H&amp;R</t>
   </si>
   <si>
     <t xml:space="preserve">Dwarka</t>
@@ -293,7 +293,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -380,10 +380,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -465,8 +461,8 @@
   </sheetPr>
   <dimension ref="A1:Z33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F33" activeCellId="0" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1008,7 +1004,6 @@
         <v>48</v>
       </c>
       <c r="G31" s="21"/>
-      <c r="H31" s="22"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">

</xml_diff>